<commit_message>
add 2C/D NMWR build functions & NMWR bug fixes
</commit_message>
<xml_diff>
--- a/NMWR Tracker.xlsx
+++ b/NMWR Tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="90">
   <si>
     <t>WP NO:</t>
   </si>
@@ -46,247 +46,244 @@
     <t>How to Use</t>
   </si>
   <si>
+    <t>Chapter 1 - General Info</t>
+  </si>
+  <si>
+    <t>G00001</t>
+  </si>
+  <si>
+    <t>General Information</t>
+  </si>
+  <si>
+    <t>G00002</t>
+  </si>
+  <si>
+    <t>Equipment Description and Data</t>
+  </si>
+  <si>
+    <t>G00003</t>
+  </si>
+  <si>
+    <t>Theory of Operation</t>
+  </si>
+  <si>
+    <t>Chapter 2 - Depot Troubleshooting Procedures</t>
+  </si>
+  <si>
+    <t>T00001</t>
+  </si>
+  <si>
+    <t>Troubleshooting Introduction</t>
+  </si>
+  <si>
+    <t>T00002</t>
+  </si>
+  <si>
+    <t>Troubleshooting Index</t>
+  </si>
+  <si>
+    <t>T00003</t>
+  </si>
+  <si>
+    <t>Preshop Analysis</t>
+  </si>
+  <si>
+    <t>T00004</t>
+  </si>
+  <si>
+    <t>Electrical Faults</t>
+  </si>
+  <si>
+    <t>T00005</t>
+  </si>
+  <si>
+    <t>Water Faults</t>
+  </si>
+  <si>
+    <t>Chapter 3 - Depot Maintenance Instructions</t>
+  </si>
+  <si>
+    <t>M00001</t>
+  </si>
+  <si>
+    <t>Preservation, Packaging and Marking General Info</t>
+  </si>
+  <si>
+    <t>M00002</t>
+  </si>
+  <si>
+    <t>Emergency Stop</t>
+  </si>
+  <si>
+    <t>Remove</t>
+  </si>
+  <si>
+    <t>M00003</t>
+  </si>
+  <si>
+    <t>Assembly</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>M00004</t>
+  </si>
+  <si>
+    <t>Install</t>
+  </si>
+  <si>
+    <t>M00005</t>
+  </si>
+  <si>
+    <t>Cargo Door</t>
+  </si>
+  <si>
+    <t>Repair</t>
+  </si>
+  <si>
+    <t>M00006</t>
+  </si>
+  <si>
+    <t>Shelter</t>
+  </si>
+  <si>
+    <t>Prepforuse</t>
+  </si>
+  <si>
+    <t>M00007</t>
+  </si>
+  <si>
+    <t>Pack</t>
+  </si>
+  <si>
+    <t>M00008</t>
+  </si>
+  <si>
+    <t>Braising Pans</t>
+  </si>
+  <si>
+    <t>Clean</t>
+  </si>
+  <si>
+    <t>M00009</t>
+  </si>
+  <si>
+    <t>Preparation For Storage</t>
+  </si>
+  <si>
+    <t>Prepstore</t>
+  </si>
+  <si>
+    <t>M00010</t>
+  </si>
+  <si>
+    <t>Preparation For Shipment</t>
+  </si>
+  <si>
+    <t>Prepship</t>
+  </si>
+  <si>
+    <t>M00011</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>M00012</t>
+  </si>
+  <si>
+    <t>Quality Assurance Requirements</t>
+  </si>
+  <si>
+    <t>Chapter 4 - Repair Parts and Special Tools List</t>
+  </si>
+  <si>
+    <t>R00001</t>
+  </si>
+  <si>
+    <t>RPSTL Introduction</t>
+  </si>
+  <si>
+    <t>R00002</t>
+  </si>
+  <si>
+    <t>Repair Parts 1</t>
+  </si>
+  <si>
+    <t>R00003</t>
+  </si>
+  <si>
+    <t>Repair Parts 2</t>
+  </si>
+  <si>
+    <t>R00004</t>
+  </si>
+  <si>
+    <t>Repair Parts 3</t>
+  </si>
+  <si>
+    <t>R00005</t>
+  </si>
+  <si>
+    <t>Bulk Items</t>
+  </si>
+  <si>
+    <t>R00006</t>
+  </si>
+  <si>
+    <t>NSN Index</t>
+  </si>
+  <si>
+    <t>R00007</t>
+  </si>
+  <si>
+    <t>Part Number Index</t>
+  </si>
+  <si>
+    <t>Chapter 5 - Supporting Information</t>
+  </si>
+  <si>
+    <t>S00001</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>S00002</t>
+  </si>
+  <si>
+    <t>Expendable and Durable Items List</t>
+  </si>
+  <si>
+    <t>S00003</t>
+  </si>
+  <si>
+    <t>Tool Identification List</t>
+  </si>
+  <si>
+    <t>S00004</t>
+  </si>
+  <si>
+    <t>Mandatory Replacement Parts</t>
+  </si>
+  <si>
+    <t>S00005</t>
+  </si>
+  <si>
+    <t>Critical Safety Items</t>
+  </si>
+  <si>
+    <t>S00006</t>
+  </si>
+  <si>
+    <t>Additional Supporting Work Packages</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Chapter 1 - General Info</t>
-  </si>
-  <si>
-    <t>G00001</t>
-  </si>
-  <si>
-    <t>General Information</t>
-  </si>
-  <si>
-    <t>G00002</t>
-  </si>
-  <si>
-    <t>Equipment Description and Data</t>
-  </si>
-  <si>
-    <t>G00003</t>
-  </si>
-  <si>
-    <t>Theory of Operation</t>
-  </si>
-  <si>
-    <t>Chapter 2 - Depot Troubleshooting Procedures</t>
-  </si>
-  <si>
-    <t>T00001</t>
-  </si>
-  <si>
-    <t>Troubleshooting Introduction</t>
-  </si>
-  <si>
-    <t>T00002</t>
-  </si>
-  <si>
-    <t>Troubleshooting Index</t>
-  </si>
-  <si>
-    <t>T00003</t>
-  </si>
-  <si>
-    <t>Preshop Analysis</t>
-  </si>
-  <si>
-    <t>T00004</t>
-  </si>
-  <si>
-    <t>Electrical Faults</t>
-  </si>
-  <si>
-    <t>T00005</t>
-  </si>
-  <si>
-    <t>Water Faults</t>
-  </si>
-  <si>
-    <t>Chapter 3 - Depot Maintenance Instructions</t>
-  </si>
-  <si>
-    <t>M00001</t>
-  </si>
-  <si>
-    <t>Preservation, Packaging and Marking General Info</t>
-  </si>
-  <si>
-    <t>M00002</t>
-  </si>
-  <si>
-    <t>Emergency Stop</t>
-  </si>
-  <si>
-    <t>Remove</t>
-  </si>
-  <si>
-    <t>M00003</t>
-  </si>
-  <si>
-    <t>Assembly</t>
-  </si>
-  <si>
-    <t>Service</t>
-  </si>
-  <si>
-    <t>M00004</t>
-  </si>
-  <si>
-    <t>Install</t>
-  </si>
-  <si>
-    <t>M00005</t>
-  </si>
-  <si>
-    <t>Cargo Door</t>
-  </si>
-  <si>
-    <t>Repair</t>
-  </si>
-  <si>
-    <t>M00006</t>
-  </si>
-  <si>
-    <t>Shelter</t>
-  </si>
-  <si>
-    <t>Prepforuse</t>
-  </si>
-  <si>
-    <t>M00007</t>
-  </si>
-  <si>
-    <t>Pack</t>
-  </si>
-  <si>
-    <t>M00008</t>
-  </si>
-  <si>
-    <t>Braising Pans</t>
-  </si>
-  <si>
-    <t>Clean</t>
-  </si>
-  <si>
-    <t>M00009</t>
-  </si>
-  <si>
-    <t>Preparation For Storage</t>
-  </si>
-  <si>
-    <t>Prepstore</t>
-  </si>
-  <si>
-    <t>M00010</t>
-  </si>
-  <si>
-    <t>Preparation For Shipment</t>
-  </si>
-  <si>
-    <t>Prepship</t>
-  </si>
-  <si>
-    <t>M00011</t>
-  </si>
-  <si>
-    <t>Transport</t>
-  </si>
-  <si>
-    <t>M00012</t>
-  </si>
-  <si>
-    <t>Quality Assurance Requirements</t>
-  </si>
-  <si>
-    <t>Chapter 4 - Repair Parts and Special Tools List</t>
-  </si>
-  <si>
-    <t>R00001</t>
-  </si>
-  <si>
-    <t>RPSTL Introduction</t>
-  </si>
-  <si>
-    <t>R00002</t>
-  </si>
-  <si>
-    <t>Repair Parts 1</t>
-  </si>
-  <si>
-    <t>R00003</t>
-  </si>
-  <si>
-    <t>Repair Parts 2</t>
-  </si>
-  <si>
-    <t>R00004</t>
-  </si>
-  <si>
-    <t>Repair Parts 3</t>
-  </si>
-  <si>
-    <t>R00005</t>
-  </si>
-  <si>
-    <t>Bulk Items</t>
-  </si>
-  <si>
-    <t>R00006</t>
-  </si>
-  <si>
-    <t>NSN Index</t>
-  </si>
-  <si>
-    <t>R00007</t>
-  </si>
-  <si>
-    <t>Part Number Index</t>
-  </si>
-  <si>
-    <t>Chapter 5 - Supporting Information</t>
-  </si>
-  <si>
-    <t>S00001</t>
-  </si>
-  <si>
-    <t>References</t>
-  </si>
-  <si>
-    <t>S00002</t>
-  </si>
-  <si>
-    <t>Expendable and Durable Items List</t>
-  </si>
-  <si>
-    <t>S00003</t>
-  </si>
-  <si>
-    <t>Tool Identification List</t>
-  </si>
-  <si>
-    <t>S00004</t>
-  </si>
-  <si>
-    <t>Mandatory Replacement Parts</t>
-  </si>
-  <si>
-    <t>S00005</t>
-  </si>
-  <si>
-    <t>Critical Safety Items</t>
-  </si>
-  <si>
-    <t>S00006</t>
-  </si>
-  <si>
-    <t>Support Items</t>
-  </si>
-  <si>
-    <t>S00007</t>
-  </si>
-  <si>
-    <t>Additional Supporting Work Packages</t>
+    <t>Rear Matter</t>
   </si>
 </sst>
 </file>
@@ -317,7 +314,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -395,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -425,9 +422,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -744,11 +738,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="55.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="55.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="10.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -821,24 +815,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="D7" s="9"/>
-      <c r="E7" s="11" t="s">
-        <v>10</v>
-      </c>
+      <c r="E7" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
       <c r="A8" s="1"/>
       <c r="B8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9" t="s">
@@ -848,10 +838,10 @@
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
       <c r="A9" s="1"/>
       <c r="B9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9" t="s">
@@ -861,21 +851,19 @@
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
       <c r="A10" s="1"/>
       <c r="B10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="B11" s="7"/>
       <c r="C11" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -883,10 +871,10 @@
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
       <c r="A12" s="1"/>
       <c r="B12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -894,23 +882,21 @@
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
       <c r="A13" s="1"/>
       <c r="B13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="D13" s="9"/>
-      <c r="E13" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="21">
+      <c r="E13" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
       <c r="A14" s="1"/>
       <c r="B14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9" t="s">
@@ -920,32 +906,30 @@
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
       <c r="A15" s="1"/>
       <c r="B15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="21">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
       <c r="A16" s="1"/>
       <c r="B16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="B17" s="7"/>
       <c r="C17" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -953,119 +937,115 @@
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
       <c r="A18" s="1"/>
       <c r="B18" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>10</v>
-      </c>
+      <c r="D18" s="9"/>
       <c r="E18" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
       <c r="A19" s="1"/>
       <c r="B19" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="D19" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="E19" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
       <c r="A20" s="1"/>
       <c r="B20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="D20" s="9" t="s">
         <v>36</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="E20" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
       <c r="A21" s="1"/>
       <c r="B21" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>39</v>
       </c>
       <c r="E21" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25">
       <c r="A22" s="1"/>
       <c r="B22" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="D22" s="9" t="s">
         <v>41</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>42</v>
       </c>
       <c r="E22" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
       <c r="A23" s="1"/>
       <c r="B23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="D23" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="E23" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25">
       <c r="A24" s="1"/>
       <c r="B24" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>47</v>
       </c>
       <c r="E24" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25">
       <c r="A25" s="1"/>
       <c r="B25" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>10</v>
-      </c>
+      <c r="E25" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="20.25">
       <c r="A26" s="1"/>
       <c r="B26" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="D26" s="9" t="s">
         <v>52</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>53</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>5</v>
@@ -1074,13 +1054,13 @@
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="20.25">
       <c r="A27" s="1"/>
       <c r="B27" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="D27" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>5</v>
@@ -1089,13 +1069,13 @@
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="20.25">
       <c r="A28" s="1"/>
       <c r="B28" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>58</v>
-      </c>
       <c r="D28" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>5</v>
@@ -1104,10 +1084,10 @@
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="20.25">
       <c r="A29" s="1"/>
       <c r="B29" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>60</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9" t="s">
@@ -1116,24 +1096,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="20.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="B30" s="7"/>
       <c r="C30" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" s="9"/>
-      <c r="E30" s="11" t="s">
-        <v>10</v>
-      </c>
+      <c r="E30" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="20.25">
       <c r="A31" s="1"/>
       <c r="B31" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9" t="s">
@@ -1143,10 +1119,10 @@
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="20.25">
       <c r="A32" s="1"/>
       <c r="B32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9" t="s">
@@ -1156,10 +1132,10 @@
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="20.25">
       <c r="A33" s="1"/>
       <c r="B33" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
@@ -1167,10 +1143,10 @@
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="20.25">
       <c r="A34" s="1"/>
       <c r="B34" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>69</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
@@ -1178,23 +1154,21 @@
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="20.25">
       <c r="A35" s="1"/>
       <c r="B35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>71</v>
-      </c>
       <c r="D35" s="9"/>
-      <c r="E35" s="11" t="s">
-        <v>10</v>
-      </c>
+      <c r="E35" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="20.25">
       <c r="A36" s="1"/>
       <c r="B36" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>73</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9" t="s">
@@ -1204,10 +1178,10 @@
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="20.25">
       <c r="A37" s="1"/>
       <c r="B37" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>75</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9" t="s">
@@ -1216,24 +1190,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="1"/>
-      <c r="B38" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="B38" s="7"/>
       <c r="C38" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D38" s="9"/>
-      <c r="E38" s="11" t="s">
-        <v>10</v>
-      </c>
+      <c r="E38" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="1"/>
       <c r="B39" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>78</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9" t="s">
@@ -1243,10 +1213,10 @@
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="1"/>
       <c r="B40" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="9" t="s">
@@ -1256,10 +1226,10 @@
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="1"/>
       <c r="B41" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9" t="s">
@@ -1269,10 +1239,10 @@
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="1"/>
       <c r="B42" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9" t="s">
@@ -1282,10 +1252,10 @@
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="1"/>
       <c r="B43" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="9" t="s">
@@ -1295,21 +1265,21 @@
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="1"/>
       <c r="B44" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>88</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="1"/>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>90</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>

</xml_diff>